<commit_message>
update vq sample data
</commit_message>
<xml_diff>
--- a/data/vq-haydn-config.xlsx
+++ b/data/vq-haydn-config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmg/workspace/music-class-chat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A44E6E-39B0-C44E-B829-C98F8C9C4169}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE842F35-774D-DE40-AC9F-E63A2B6722BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="8" xr2:uid="{E8A503D0-EC5A-E746-BAA9-7113C281CDDE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="3" xr2:uid="{E8A503D0-EC5A-E746-BAA9-7113C281CDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="222">
   <si>
     <t>name</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>hidden; given when intro complete</t>
-  </si>
-  <si>
-    <t>bell</t>
   </si>
   <si>
     <t>bell.png</t>
@@ -318,9 +315,6 @@
     <t>finished element</t>
   </si>
   <si>
-    <t>a bell. For something. Just an example</t>
-  </si>
-  <si>
     <t>1. Harmophony</t>
   </si>
   <si>
@@ -363,25 +357,10 @@
     <t>Choose one of these musical examples:</t>
   </si>
   <si>
-    <t>1. Haydn - “Fifths” Quartet in D minor, Op. 76, No. 2</t>
-  </si>
-  <si>
     <t>…</t>
   </si>
   <si>
     <t>examples</t>
-  </si>
-  <si>
-    <t>2. Ethel Smyth - Quartet in E minor</t>
-  </si>
-  <si>
-    <t>3. Felix Mendelssohn - Quartet in A minor, Op. 13</t>
-  </si>
-  <si>
-    <t>4. Wynton Marsalis - String Quartet No. 1 “At the Octoroon Balls”</t>
-  </si>
-  <si>
-    <t>Let’s find out more about Haydn -  “Fifths” Quartet in D minor, Op. 76, No. 2!</t>
   </si>
   <si>
     <t>example1</t>
@@ -393,13 +372,7 @@
     <t>See the Musical Score</t>
   </si>
   <si>
-    <t>Franz Josef Haydn  (1732-1809)</t>
-  </si>
-  <si>
     <t>example1score</t>
-  </si>
-  <si>
-    <t>[animation of score]</t>
   </si>
   <si>
     <t>This Menuetto is the third movement of Haydn’s quartet, and is in 3/4 time.</t>
@@ -596,6 +569,147 @@
   <si>
     <t>doingel1,doingel2,doingel3,doingel4</t>
   </si>
+  <si>
+    <t>example4</t>
+  </si>
+  <si>
+    <t>el2ex4score,el2ex4video,el2ex4bio</t>
+  </si>
+  <si>
+    <t>el2ex4video</t>
+  </si>
+  <si>
+    <t>el2ex4score</t>
+  </si>
+  <si>
+    <t>el2ex4bio</t>
+  </si>
+  <si>
+    <t>example4score</t>
+  </si>
+  <si>
+    <t>Haydn - “Fifths” Quartet in D minor, Op. 76, No. 2: COUNTERPOINT IN ROUND</t>
+  </si>
+  <si>
+    <t>Ethel Smyth - Quartet in E minor: FAST FUGUE</t>
+  </si>
+  <si>
+    <t>Felix Mendelssohn - Quartet in A minor, Op. 13: SLOW FUGUE</t>
+  </si>
+  <si>
+    <t>Wynton Marsalis - String Quartet No. 1 “At the Octoroon Balls”: CALL &amp; RESPONSE</t>
+  </si>
+  <si>
+    <t>FRANZ JOSEPH HAYDN (1732 - 1809) - COUNTERPOINT IN ROUND</t>
+  </si>
+  <si>
+    <t>Let’s find out more about Haydn - “Fifths” Quartet in D minor, Op. 76, No. 2!</t>
+  </si>
+  <si>
+    <t>Haydn - Quartet in D minor "Fifths" Op. 76, No. 2. 3rd movement – Menuetto</t>
+  </si>
+  <si>
+    <t>example1video</t>
+  </si>
+  <si>
+    <t>https://youtu.be/iVm_Mw0F6aA</t>
+  </si>
+  <si>
+    <t>When the quartet is split in two, can you hear the two lines separately?</t>
+  </si>
+  <si>
+    <t>About Franz Josef Haydn (1732 - 1809)</t>
+  </si>
+  <si>
+    <t>example1bio</t>
+  </si>
+  <si>
+    <t>[image of haydn]</t>
+  </si>
+  <si>
+    <t>Franz Joseph Haydn is known as the “Father of the String Quartet.” He wrote 68 string quartets and was the first composer to define the genre of string quartet in European musical culture. He was born in Austria and was amazingly popular during his lifetime.</t>
+  </si>
+  <si>
+    <t>The six string quartets from his Op. 76 collection were composed in 1797 and dedicated to the Hungarian count Joseph Georg von Erdody. Usually big works would be commissioned by someone with plenty of money - they take a lot of time and effort and would have been quite expensive!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How many quartets did Haydn write? </t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>example1bioquiz</t>
+  </si>
+  <si>
+    <t>WYNTON MARSALIS (born 1961) - CALL &amp; RESPONSE</t>
+  </si>
+  <si>
+    <t>Let’s learn about Marsalis - String Quartet No.1 "At the Octoroon Balls"!</t>
+  </si>
+  <si>
+    <t>example4video</t>
+  </si>
+  <si>
+    <t>Marsalis - String Quartet No. 1 “At the Octoroon Balls”. 4th Movement, “Many Gone” (excerpt)</t>
+  </si>
+  <si>
+    <t>https://youtu.be/B5fgNgNvHug</t>
+  </si>
+  <si>
+    <t>How would you describe the rhythms in this excerpt and what do they remind you of?</t>
+  </si>
+  <si>
+    <t>[TO DO FREE TEXT]</t>
+  </si>
+  <si>
+    <t>example4bio</t>
+  </si>
+  <si>
+    <t>About Wynton Marsalis (b. 1961)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wynton Marsalis was born on October 18, 1961 in New Orleans, Louisiana. He is an American trumpeter, composer, and director of Jazz at Lincoln Center. He is a successful artist in both the classical and jazz realms, having performed as a soloist with leading orchestras including the New York Philharmonic, the Los Angeles Philharmonic, and the English Chamber Orchestra. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In many of his compositions, he combines the structures of classical music with jazz and blues. </t>
+  </si>
+  <si>
+    <t>Marsalis has won many accolades for his compositions, including numerous Grammy Awards and the Pulitzer Prize for Music. He is the only musician to win a Grammy Award in both the jazz and classical categories during the same year.</t>
+  </si>
+  <si>
+    <t>Where was Wynton Marsalis born?</t>
+  </si>
+  <si>
+    <t>example4bioquiz</t>
+  </si>
+  <si>
+    <t>New York, New York</t>
+  </si>
+  <si>
+    <t>Los Angeles, California</t>
+  </si>
+  <si>
+    <t>New Orleans, Louisiana</t>
+  </si>
+  <si>
+    <t>This excerpt from the 4th movement is a demonstration of ‘call and response.’ This is counterpoint in perhaps its simplest form - one voice reacting to another. The viola makes a proud declaration, and it’s followed by a collective and emphatic response from the others in the quartet.</t>
+  </si>
+  <si>
+    <t>Can you see how Marsalis has taken inspiration from songs and American spirituals in this quartet? You can see the words “On my knees but I didn’t pray”.</t>
+  </si>
+  <si>
+    <t>upload/vq/haydn_fifths_score.jpg</t>
+  </si>
+  <si>
+    <t>upload/vq/marsalis_manygone_score.png</t>
+  </si>
 </sst>
 </file>
 
@@ -657,29 +771,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="142">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -1091,6 +1190,21 @@
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1124,39 +1238,39 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{001E279C-34E1-6C4C-831C-2EFE910D8A17}" name="Table88" displayName="Table88" ref="A1:Q25" totalsRowShown="0" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{001E279C-34E1-6C4C-831C-2EFE910D8A17}" name="Table88" displayName="Table88" ref="A1:Q25" totalsRowShown="0" dataDxfId="17">
   <autoFilter ref="A1:Q25" xr:uid="{669026F6-523A-EF49-B01A-F3286CFBC418}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{6E3EFBA6-A4F0-8848-814B-DB2A8B42A028}" name="label" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{26F28EF1-4977-104E-84BF-6CDB8C592B86}" name="ifall" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{6EA01476-596D-0B41-BDBA-09C71887F06D}" name="andnot" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{D5CE29D5-0B29-6E4B-960B-6E82925D1012}" name="after" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{615CE360-56E4-E74E-A4FE-581A6667718F}" name="waitfor" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{0F6403CB-723D-3240-8E44-099B19A2A0BB}" name="ornext" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{D7B5D7A5-5968-764E-8BCD-B45F9543127B}" name="message" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{B0D60912-AF1B-5E4E-87BA-2BE9C34E10FC}" name="type" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{6C67A1A5-16A7-E34A-9940-5F76CAF3CDA2}" name="url" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{CAC35FA8-F0A9-D049-BAC3-6886EE4C49FA}" name="title" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{F88EA64A-2C49-AE4F-BD3A-89DC9D9BEC0B}" name="description" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{D4DEB4AD-B42E-9A4B-AF66-E97A3D8DC2AF}" name="section" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{C690E6CB-01CD-EA41-8AF5-0FCFE7454D59}" name="sortorder" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{E9FC5C6F-9A36-6C45-A6D4-A94D1CB8E5E0}" name="hidden" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{FE15E9B1-1807-2140-97E1-59931B3BB0B3}" name="rewards" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{38B48344-8937-514C-AD97-D7065729C3DD}" name="reset" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{EE123146-76E6-6147-8BC2-698DC2B5F5AC}" name="jumpto" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{6E3EFBA6-A4F0-8848-814B-DB2A8B42A028}" name="label" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{26F28EF1-4977-104E-84BF-6CDB8C592B86}" name="ifall" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{6EA01476-596D-0B41-BDBA-09C71887F06D}" name="andnot" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{D5CE29D5-0B29-6E4B-960B-6E82925D1012}" name="after" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{615CE360-56E4-E74E-A4FE-581A6667718F}" name="waitfor" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{0F6403CB-723D-3240-8E44-099B19A2A0BB}" name="ornext" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{D7B5D7A5-5968-764E-8BCD-B45F9543127B}" name="message" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{B0D60912-AF1B-5E4E-87BA-2BE9C34E10FC}" name="type" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{6C67A1A5-16A7-E34A-9940-5F76CAF3CDA2}" name="url" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{CAC35FA8-F0A9-D049-BAC3-6886EE4C49FA}" name="title" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{F88EA64A-2C49-AE4F-BD3A-89DC9D9BEC0B}" name="description" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{D4DEB4AD-B42E-9A4B-AF66-E97A3D8DC2AF}" name="section" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{C690E6CB-01CD-EA41-8AF5-0FCFE7454D59}" name="sortorder" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{E9FC5C6F-9A36-6C45-A6D4-A94D1CB8E5E0}" name="hidden" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{FE15E9B1-1807-2140-97E1-59931B3BB0B3}" name="rewards" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{38B48344-8937-514C-AD97-D7065729C3DD}" name="reset" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{EE123146-76E6-6147-8BC2-698DC2B5F5AC}" name="jumpto" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC33DAED-8B40-2544-B087-DDF69FF66ECC}" name="Table3" displayName="Table3" ref="A1:D29" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="A1:D29" xr:uid="{A0226A79-3B4F-CE40-8B64-1DAFAD80F509}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC33DAED-8B40-2544-B087-DDF69FF66ECC}" name="Table3" displayName="Table3" ref="A1:D31" totalsRowShown="0" dataDxfId="137">
+  <autoFilter ref="A1:D31" xr:uid="{A0226A79-3B4F-CE40-8B64-1DAFAD80F509}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B1952672-FA76-8244-A817-C7FF5E7BBCC3}" name="_id" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{A4BABDC0-8353-104D-9897-1182219AA6E9}" name="icon" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{295BA006-D777-C94C-9A3B-CBCE6DFA30F7}" name="noicon" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{6DB67210-B9D7-984E-9299-85DD07F56828}" name="comment" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B1952672-FA76-8244-A817-C7FF5E7BBCC3}" name="_id" dataDxfId="136"/>
+    <tableColumn id="2" xr3:uid="{A4BABDC0-8353-104D-9897-1182219AA6E9}" name="icon" dataDxfId="135"/>
+    <tableColumn id="3" xr3:uid="{295BA006-D777-C94C-9A3B-CBCE6DFA30F7}" name="noicon" dataDxfId="134"/>
+    <tableColumn id="4" xr3:uid="{6DB67210-B9D7-984E-9299-85DD07F56828}" name="comment" dataDxfId="133"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1166,169 +1280,169 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{46CC7FC3-C398-E54A-8F0F-67C0FFA584F9}" name="Table6" displayName="Table6" ref="A1:G8" totalsRowShown="0">
   <autoFilter ref="A1:G8" xr:uid="{E6246C16-1458-2446-86A3-56CB4DDF4212}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{14EACF44-C26D-C241-8D88-1DC9DB8FCF0D}" name="name" dataDxfId="137"/>
-    <tableColumn id="7" xr3:uid="{7246BEBC-13A8-EB46-90C3-1EA396465A79}" name="_id" dataDxfId="136"/>
-    <tableColumn id="2" xr3:uid="{89511BC0-8A83-6245-BB1D-AA3BBE172266}" name="description" dataDxfId="135"/>
-    <tableColumn id="3" xr3:uid="{942A6288-00A2-5544-B50C-650370B9F125}" name="icon" dataDxfId="134"/>
-    <tableColumn id="4" xr3:uid="{2185EE55-A940-F946-A627-49D344ED51AB}" name="sortorder" dataDxfId="133"/>
-    <tableColumn id="5" xr3:uid="{D03B7F16-DD48-D044-9A94-387DF9E748D4}" name="ifall" dataDxfId="132"/>
-    <tableColumn id="6" xr3:uid="{ADE9A9F1-7512-7E41-924F-A2B8D11FB01C}" name="andnot" dataDxfId="131"/>
+    <tableColumn id="1" xr3:uid="{14EACF44-C26D-C241-8D88-1DC9DB8FCF0D}" name="name" dataDxfId="132"/>
+    <tableColumn id="7" xr3:uid="{7246BEBC-13A8-EB46-90C3-1EA396465A79}" name="_id" dataDxfId="131"/>
+    <tableColumn id="2" xr3:uid="{89511BC0-8A83-6245-BB1D-AA3BBE172266}" name="description" dataDxfId="130"/>
+    <tableColumn id="3" xr3:uid="{942A6288-00A2-5544-B50C-650370B9F125}" name="icon" dataDxfId="129"/>
+    <tableColumn id="4" xr3:uid="{2185EE55-A940-F946-A627-49D344ED51AB}" name="sortorder" dataDxfId="128"/>
+    <tableColumn id="5" xr3:uid="{D03B7F16-DD48-D044-9A94-387DF9E748D4}" name="ifall" dataDxfId="127"/>
+    <tableColumn id="6" xr3:uid="{ADE9A9F1-7512-7E41-924F-A2B8D11FB01C}" name="andnot" dataDxfId="126"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D5C0D842-BB95-3948-9E74-73C8655AA488}" name="Table8" displayName="Table8" ref="A1:Q25" totalsRowShown="0" dataDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D5C0D842-BB95-3948-9E74-73C8655AA488}" name="Table8" displayName="Table8" ref="A1:Q25" totalsRowShown="0" dataDxfId="125">
   <autoFilter ref="A1:Q25" xr:uid="{669026F6-523A-EF49-B01A-F3286CFBC418}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{98209BBC-74B8-0C48-8788-C46719605874}" name="label" dataDxfId="129"/>
-    <tableColumn id="2" xr3:uid="{67E33C65-F324-5447-9B5E-CD7DEA820D5F}" name="ifall" dataDxfId="128"/>
-    <tableColumn id="3" xr3:uid="{96F4C912-DDCB-9343-ABC8-65914498E850}" name="andnot" dataDxfId="127"/>
-    <tableColumn id="4" xr3:uid="{3C49259E-D837-304B-AEF0-D0E2D9F1CFFF}" name="after" dataDxfId="126"/>
-    <tableColumn id="5" xr3:uid="{BD167AE1-ADDC-D34F-A91C-94AA598E624A}" name="waitfor" dataDxfId="125"/>
-    <tableColumn id="6" xr3:uid="{BE72769F-64DC-AE49-A803-DDC74261D522}" name="ornext" dataDxfId="124"/>
-    <tableColumn id="7" xr3:uid="{3D9CBAD6-6312-FF40-B0BA-D5463A6E6774}" name="message" dataDxfId="123"/>
-    <tableColumn id="8" xr3:uid="{1BE9E1EF-0CDE-E84E-993D-DE2429DEF690}" name="type" dataDxfId="122"/>
-    <tableColumn id="9" xr3:uid="{2F612D43-F908-6E4E-8D31-EC869F33F6E9}" name="url" dataDxfId="121"/>
-    <tableColumn id="10" xr3:uid="{8A769766-7E92-F748-BAB6-502136570385}" name="title" dataDxfId="120"/>
-    <tableColumn id="11" xr3:uid="{84647AA4-DC4E-6042-938A-8DD06D6FEE16}" name="description" dataDxfId="119"/>
-    <tableColumn id="12" xr3:uid="{4C0CC8EC-5DF9-EF40-A394-04179633987D}" name="section" dataDxfId="118"/>
-    <tableColumn id="13" xr3:uid="{3EC412FF-9AC2-D14B-8F4E-F9DBD3BA4519}" name="sortorder" dataDxfId="117"/>
-    <tableColumn id="14" xr3:uid="{3519660E-5EAF-8D4D-8894-76FFA8BA0976}" name="hidden" dataDxfId="116"/>
-    <tableColumn id="15" xr3:uid="{7E07B26D-13A3-0444-AC8A-C296741EFB75}" name="rewards" dataDxfId="115"/>
-    <tableColumn id="16" xr3:uid="{817F2933-35C9-4C45-AA59-74EB42A0D73E}" name="reset" dataDxfId="114"/>
-    <tableColumn id="17" xr3:uid="{8B62FD90-4BF1-0D40-843E-3CA898042B40}" name="jumpto" dataDxfId="113"/>
+    <tableColumn id="1" xr3:uid="{98209BBC-74B8-0C48-8788-C46719605874}" name="label" dataDxfId="124"/>
+    <tableColumn id="2" xr3:uid="{67E33C65-F324-5447-9B5E-CD7DEA820D5F}" name="ifall" dataDxfId="123"/>
+    <tableColumn id="3" xr3:uid="{96F4C912-DDCB-9343-ABC8-65914498E850}" name="andnot" dataDxfId="122"/>
+    <tableColumn id="4" xr3:uid="{3C49259E-D837-304B-AEF0-D0E2D9F1CFFF}" name="after" dataDxfId="121"/>
+    <tableColumn id="5" xr3:uid="{BD167AE1-ADDC-D34F-A91C-94AA598E624A}" name="waitfor" dataDxfId="120"/>
+    <tableColumn id="6" xr3:uid="{BE72769F-64DC-AE49-A803-DDC74261D522}" name="ornext" dataDxfId="119"/>
+    <tableColumn id="7" xr3:uid="{3D9CBAD6-6312-FF40-B0BA-D5463A6E6774}" name="message" dataDxfId="118"/>
+    <tableColumn id="8" xr3:uid="{1BE9E1EF-0CDE-E84E-993D-DE2429DEF690}" name="type" dataDxfId="117"/>
+    <tableColumn id="9" xr3:uid="{2F612D43-F908-6E4E-8D31-EC869F33F6E9}" name="url" dataDxfId="116"/>
+    <tableColumn id="10" xr3:uid="{8A769766-7E92-F748-BAB6-502136570385}" name="title" dataDxfId="115"/>
+    <tableColumn id="11" xr3:uid="{84647AA4-DC4E-6042-938A-8DD06D6FEE16}" name="description" dataDxfId="114"/>
+    <tableColumn id="12" xr3:uid="{4C0CC8EC-5DF9-EF40-A394-04179633987D}" name="section" dataDxfId="113"/>
+    <tableColumn id="13" xr3:uid="{3EC412FF-9AC2-D14B-8F4E-F9DBD3BA4519}" name="sortorder" dataDxfId="112"/>
+    <tableColumn id="14" xr3:uid="{3519660E-5EAF-8D4D-8894-76FFA8BA0976}" name="hidden" dataDxfId="111"/>
+    <tableColumn id="15" xr3:uid="{7E07B26D-13A3-0444-AC8A-C296741EFB75}" name="rewards" dataDxfId="110"/>
+    <tableColumn id="16" xr3:uid="{817F2933-35C9-4C45-AA59-74EB42A0D73E}" name="reset" dataDxfId="109"/>
+    <tableColumn id="17" xr3:uid="{8B62FD90-4BF1-0D40-843E-3CA898042B40}" name="jumpto" dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0B2A40C4-7877-474D-AF59-BB042BA0FC6D}" name="Table810" displayName="Table810" ref="A1:Q23" totalsRowShown="0" dataDxfId="112">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0B2A40C4-7877-474D-AF59-BB042BA0FC6D}" name="Table810" displayName="Table810" ref="A1:Q23" totalsRowShown="0" dataDxfId="107">
   <autoFilter ref="A1:Q23" xr:uid="{669026F6-523A-EF49-B01A-F3286CFBC418}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{2B440253-680B-2247-B853-0979AE53EDD8}" name="label" dataDxfId="111"/>
-    <tableColumn id="2" xr3:uid="{1A484451-0875-C749-B2F5-7E5897DE5603}" name="ifall" dataDxfId="110"/>
-    <tableColumn id="3" xr3:uid="{104A9865-E04C-3147-8C1B-4E4F83F04636}" name="andnot" dataDxfId="109"/>
-    <tableColumn id="4" xr3:uid="{56115264-3302-2542-81BE-FF30A56B9C54}" name="after" dataDxfId="108"/>
-    <tableColumn id="5" xr3:uid="{A294F377-14F0-D94F-88EB-910B6B34D824}" name="waitfor" dataDxfId="107"/>
-    <tableColumn id="6" xr3:uid="{936A0470-DEF3-8247-A24D-428C870F35E0}" name="ornext" dataDxfId="106"/>
-    <tableColumn id="7" xr3:uid="{7BFBE5EC-8CDB-0644-9EC0-AAEF93718DFB}" name="message" dataDxfId="105"/>
-    <tableColumn id="8" xr3:uid="{0FEACC26-B678-8944-A462-ADB539D13642}" name="type" dataDxfId="104"/>
-    <tableColumn id="9" xr3:uid="{0D022D26-1092-FF45-A0D8-CC149074B846}" name="url" dataDxfId="103"/>
-    <tableColumn id="10" xr3:uid="{19BDB18B-88B7-9E48-A2FE-488E75BA84C2}" name="title" dataDxfId="102"/>
-    <tableColumn id="11" xr3:uid="{AB56076E-698E-D841-8B1A-622FF0DB045F}" name="description" dataDxfId="101"/>
-    <tableColumn id="12" xr3:uid="{48ABAADE-729A-7843-BA82-8F26C2542086}" name="section" dataDxfId="100"/>
-    <tableColumn id="13" xr3:uid="{D7B394A7-C4A0-1A4A-A1E7-AD17CB0589A8}" name="sortorder" dataDxfId="99"/>
-    <tableColumn id="14" xr3:uid="{1CADD3D5-7424-074A-B60C-904978AE200C}" name="hidden" dataDxfId="98"/>
-    <tableColumn id="15" xr3:uid="{4ADA220A-13B5-B048-9C88-1C06EBC9D22C}" name="rewards" dataDxfId="97"/>
-    <tableColumn id="16" xr3:uid="{5CA885B2-6C6B-8E43-9687-61B995EBBD98}" name="reset" dataDxfId="96"/>
-    <tableColumn id="17" xr3:uid="{2E3DD60E-38B7-FD44-AC56-FEB0F8BFFDB9}" name="jumpto" dataDxfId="95"/>
+    <tableColumn id="1" xr3:uid="{2B440253-680B-2247-B853-0979AE53EDD8}" name="label" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{1A484451-0875-C749-B2F5-7E5897DE5603}" name="ifall" dataDxfId="105"/>
+    <tableColumn id="3" xr3:uid="{104A9865-E04C-3147-8C1B-4E4F83F04636}" name="andnot" dataDxfId="104"/>
+    <tableColumn id="4" xr3:uid="{56115264-3302-2542-81BE-FF30A56B9C54}" name="after" dataDxfId="103"/>
+    <tableColumn id="5" xr3:uid="{A294F377-14F0-D94F-88EB-910B6B34D824}" name="waitfor" dataDxfId="102"/>
+    <tableColumn id="6" xr3:uid="{936A0470-DEF3-8247-A24D-428C870F35E0}" name="ornext" dataDxfId="101"/>
+    <tableColumn id="7" xr3:uid="{7BFBE5EC-8CDB-0644-9EC0-AAEF93718DFB}" name="message" dataDxfId="100"/>
+    <tableColumn id="8" xr3:uid="{0FEACC26-B678-8944-A462-ADB539D13642}" name="type" dataDxfId="99"/>
+    <tableColumn id="9" xr3:uid="{0D022D26-1092-FF45-A0D8-CC149074B846}" name="url" dataDxfId="98"/>
+    <tableColumn id="10" xr3:uid="{19BDB18B-88B7-9E48-A2FE-488E75BA84C2}" name="title" dataDxfId="97"/>
+    <tableColumn id="11" xr3:uid="{AB56076E-698E-D841-8B1A-622FF0DB045F}" name="description" dataDxfId="96"/>
+    <tableColumn id="12" xr3:uid="{48ABAADE-729A-7843-BA82-8F26C2542086}" name="section" dataDxfId="95"/>
+    <tableColumn id="13" xr3:uid="{D7B394A7-C4A0-1A4A-A1E7-AD17CB0589A8}" name="sortorder" dataDxfId="94"/>
+    <tableColumn id="14" xr3:uid="{1CADD3D5-7424-074A-B60C-904978AE200C}" name="hidden" dataDxfId="93"/>
+    <tableColumn id="15" xr3:uid="{4ADA220A-13B5-B048-9C88-1C06EBC9D22C}" name="rewards" dataDxfId="92"/>
+    <tableColumn id="16" xr3:uid="{5CA885B2-6C6B-8E43-9687-61B995EBBD98}" name="reset" dataDxfId="91"/>
+    <tableColumn id="17" xr3:uid="{2E3DD60E-38B7-FD44-AC56-FEB0F8BFFDB9}" name="jumpto" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97C05CA8-913E-2240-AF00-ACE7860C25D2}" name="Table81011" displayName="Table81011" ref="A1:Q28" totalsRowShown="0" dataDxfId="94">
-  <autoFilter ref="A1:Q28" xr:uid="{669026F6-523A-EF49-B01A-F3286CFBC418}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97C05CA8-913E-2240-AF00-ACE7860C25D2}" name="Table81011" displayName="Table81011" ref="A1:Q59" totalsRowShown="0" dataDxfId="89">
+  <autoFilter ref="A1:Q59" xr:uid="{669026F6-523A-EF49-B01A-F3286CFBC418}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{014A9763-B087-2B4B-93D7-75431119447F}" name="label" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{A4F9E4B9-5020-3C48-8665-3E8315A0B800}" name="ifall" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{1C7E0588-7912-3944-B0E6-43A61005CDCE}" name="andnot" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{8989FA64-7FB9-C247-B9BF-20B65C4D95A2}" name="after" dataDxfId="90"/>
-    <tableColumn id="5" xr3:uid="{62F0408F-976B-8D45-A227-44C809DD9B35}" name="waitfor" dataDxfId="89"/>
-    <tableColumn id="6" xr3:uid="{A72246FC-95B5-7746-85BD-39E49FE857EF}" name="ornext" dataDxfId="88"/>
-    <tableColumn id="7" xr3:uid="{1CB87543-7FEE-464F-B329-C58A29625D94}" name="message" dataDxfId="87"/>
-    <tableColumn id="8" xr3:uid="{05DA1C54-AE4B-D24D-9360-B6E0EE37D865}" name="type" dataDxfId="86"/>
-    <tableColumn id="9" xr3:uid="{A498DA27-4109-B34B-A2AE-B2B47AA9376F}" name="url" dataDxfId="85"/>
-    <tableColumn id="10" xr3:uid="{A44C8647-66DB-574E-974A-54DC42A0394F}" name="title" dataDxfId="84"/>
-    <tableColumn id="11" xr3:uid="{116F4944-FAF5-1B4A-94BC-EF69D91BB31F}" name="description" dataDxfId="83"/>
-    <tableColumn id="12" xr3:uid="{63D38E18-E427-0E4F-8896-96FBAEFE303D}" name="section" dataDxfId="82"/>
-    <tableColumn id="13" xr3:uid="{3E26E2C5-6A81-4A42-9801-75F4DCAE94DD}" name="sortorder" dataDxfId="81"/>
-    <tableColumn id="14" xr3:uid="{45B6A2D2-7510-174B-B316-E6B99B21CA61}" name="hidden" dataDxfId="80"/>
-    <tableColumn id="15" xr3:uid="{07A739DF-1EF3-C84D-A0AA-5AC780A62237}" name="rewards" dataDxfId="79"/>
-    <tableColumn id="16" xr3:uid="{1A794E51-2011-174A-94E7-B84BDA0472FE}" name="reset" dataDxfId="78"/>
-    <tableColumn id="17" xr3:uid="{BE08941E-FE4B-484F-9017-CAA09458CEFB}" name="jumpto" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{014A9763-B087-2B4B-93D7-75431119447F}" name="label" dataDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{A4F9E4B9-5020-3C48-8665-3E8315A0B800}" name="ifall" dataDxfId="87"/>
+    <tableColumn id="3" xr3:uid="{1C7E0588-7912-3944-B0E6-43A61005CDCE}" name="andnot" dataDxfId="86"/>
+    <tableColumn id="4" xr3:uid="{8989FA64-7FB9-C247-B9BF-20B65C4D95A2}" name="after" dataDxfId="85"/>
+    <tableColumn id="5" xr3:uid="{62F0408F-976B-8D45-A227-44C809DD9B35}" name="waitfor" dataDxfId="84"/>
+    <tableColumn id="6" xr3:uid="{A72246FC-95B5-7746-85BD-39E49FE857EF}" name="ornext" dataDxfId="83"/>
+    <tableColumn id="7" xr3:uid="{1CB87543-7FEE-464F-B329-C58A29625D94}" name="message" dataDxfId="82"/>
+    <tableColumn id="8" xr3:uid="{05DA1C54-AE4B-D24D-9360-B6E0EE37D865}" name="type" dataDxfId="81"/>
+    <tableColumn id="9" xr3:uid="{A498DA27-4109-B34B-A2AE-B2B47AA9376F}" name="url" dataDxfId="80"/>
+    <tableColumn id="10" xr3:uid="{A44C8647-66DB-574E-974A-54DC42A0394F}" name="title" dataDxfId="79"/>
+    <tableColumn id="11" xr3:uid="{116F4944-FAF5-1B4A-94BC-EF69D91BB31F}" name="description" dataDxfId="78"/>
+    <tableColumn id="12" xr3:uid="{63D38E18-E427-0E4F-8896-96FBAEFE303D}" name="section" dataDxfId="77"/>
+    <tableColumn id="13" xr3:uid="{3E26E2C5-6A81-4A42-9801-75F4DCAE94DD}" name="sortorder" dataDxfId="76"/>
+    <tableColumn id="14" xr3:uid="{45B6A2D2-7510-174B-B316-E6B99B21CA61}" name="hidden" dataDxfId="75"/>
+    <tableColumn id="15" xr3:uid="{07A739DF-1EF3-C84D-A0AA-5AC780A62237}" name="rewards" dataDxfId="74"/>
+    <tableColumn id="16" xr3:uid="{1A794E51-2011-174A-94E7-B84BDA0472FE}" name="reset" dataDxfId="73"/>
+    <tableColumn id="17" xr3:uid="{BE08941E-FE4B-484F-9017-CAA09458CEFB}" name="jumpto" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0694DBC8-0709-3E48-A361-1482C457893D}" name="Table8102" displayName="Table8102" ref="A1:Q23" totalsRowShown="0" dataDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0694DBC8-0709-3E48-A361-1482C457893D}" name="Table8102" displayName="Table8102" ref="A1:Q23" totalsRowShown="0" dataDxfId="71">
   <autoFilter ref="A1:Q23" xr:uid="{669026F6-523A-EF49-B01A-F3286CFBC418}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{7B5D2131-B0B4-0040-B704-D6201A7C5C60}" name="label" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{324BC400-C8F1-DB49-8B88-FBCC1B6B63EA}" name="ifall" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{62A3FFD3-DF12-AB46-B499-FBD7E00E9F90}" name="andnot" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{99C835BF-C902-C94F-B072-2CF7C8C67571}" name="after" dataDxfId="72"/>
-    <tableColumn id="5" xr3:uid="{A9E9D403-CA6F-FF40-BE71-9886D4A50830}" name="waitfor" dataDxfId="71"/>
-    <tableColumn id="6" xr3:uid="{0A24648C-6E03-5345-B8CA-939736CF4517}" name="ornext" dataDxfId="70"/>
-    <tableColumn id="7" xr3:uid="{25A94D98-FF33-7E42-8FD8-ABC4D7736A34}" name="message" dataDxfId="69"/>
-    <tableColumn id="8" xr3:uid="{9AB7DC33-A3F7-9B40-A57B-F502B98AD722}" name="type" dataDxfId="68"/>
-    <tableColumn id="9" xr3:uid="{A2CD65DF-76CB-4B48-8835-680AA2485AAB}" name="url" dataDxfId="67"/>
-    <tableColumn id="10" xr3:uid="{066AF89A-F6F0-1046-9227-560DEF0CBBE9}" name="title" dataDxfId="66"/>
-    <tableColumn id="11" xr3:uid="{9112E3CC-1756-D842-AADF-FD73F6F4926D}" name="description" dataDxfId="65"/>
-    <tableColumn id="12" xr3:uid="{417D06B7-7C7C-FD44-A76D-23DBA81BE9C6}" name="section" dataDxfId="64"/>
-    <tableColumn id="13" xr3:uid="{026E2333-D133-CD4F-87B4-82D93C37D1A7}" name="sortorder" dataDxfId="63"/>
-    <tableColumn id="14" xr3:uid="{DD1C937B-1C15-9244-906F-F403CA1111D0}" name="hidden" dataDxfId="62"/>
-    <tableColumn id="15" xr3:uid="{5F34B58B-5DCC-564D-9230-A9CB31B31624}" name="rewards" dataDxfId="61"/>
-    <tableColumn id="16" xr3:uid="{FE796018-978D-F145-9CC0-32A9D248BC77}" name="reset" dataDxfId="60"/>
-    <tableColumn id="17" xr3:uid="{BAAAC35F-07CD-F44C-B7BC-84BE70C03AF8}" name="jumpto" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{7B5D2131-B0B4-0040-B704-D6201A7C5C60}" name="label" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{324BC400-C8F1-DB49-8B88-FBCC1B6B63EA}" name="ifall" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{62A3FFD3-DF12-AB46-B499-FBD7E00E9F90}" name="andnot" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{99C835BF-C902-C94F-B072-2CF7C8C67571}" name="after" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{A9E9D403-CA6F-FF40-BE71-9886D4A50830}" name="waitfor" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{0A24648C-6E03-5345-B8CA-939736CF4517}" name="ornext" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{25A94D98-FF33-7E42-8FD8-ABC4D7736A34}" name="message" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{9AB7DC33-A3F7-9B40-A57B-F502B98AD722}" name="type" dataDxfId="63"/>
+    <tableColumn id="9" xr3:uid="{A2CD65DF-76CB-4B48-8835-680AA2485AAB}" name="url" dataDxfId="62"/>
+    <tableColumn id="10" xr3:uid="{066AF89A-F6F0-1046-9227-560DEF0CBBE9}" name="title" dataDxfId="61"/>
+    <tableColumn id="11" xr3:uid="{9112E3CC-1756-D842-AADF-FD73F6F4926D}" name="description" dataDxfId="60"/>
+    <tableColumn id="12" xr3:uid="{417D06B7-7C7C-FD44-A76D-23DBA81BE9C6}" name="section" dataDxfId="59"/>
+    <tableColumn id="13" xr3:uid="{026E2333-D133-CD4F-87B4-82D93C37D1A7}" name="sortorder" dataDxfId="58"/>
+    <tableColumn id="14" xr3:uid="{DD1C937B-1C15-9244-906F-F403CA1111D0}" name="hidden" dataDxfId="57"/>
+    <tableColumn id="15" xr3:uid="{5F34B58B-5DCC-564D-9230-A9CB31B31624}" name="rewards" dataDxfId="56"/>
+    <tableColumn id="16" xr3:uid="{FE796018-978D-F145-9CC0-32A9D248BC77}" name="reset" dataDxfId="55"/>
+    <tableColumn id="17" xr3:uid="{BAAAC35F-07CD-F44C-B7BC-84BE70C03AF8}" name="jumpto" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9DB6EF27-77E9-A043-A8A9-973C58CE0D87}" name="Table8105" displayName="Table8105" ref="A1:Q23" totalsRowShown="0" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9DB6EF27-77E9-A043-A8A9-973C58CE0D87}" name="Table8105" displayName="Table8105" ref="A1:Q23" totalsRowShown="0" dataDxfId="53">
   <autoFilter ref="A1:Q23" xr:uid="{669026F6-523A-EF49-B01A-F3286CFBC418}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{A9CB85C2-9EE9-E943-8583-198E332FFDDB}" name="label" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{ECEF0727-201A-294E-BD26-4AC0074C4525}" name="ifall" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{98DC9DDF-BDE6-8E4B-A641-1CA50F97B95E}" name="andnot" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{8BFB331E-5056-234D-86A1-1CBB34D2A4A4}" name="after" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{F7D28942-23E3-544B-AE2F-F73BE9CE5841}" name="waitfor" dataDxfId="53"/>
-    <tableColumn id="6" xr3:uid="{DE531C20-A3B2-5C46-A368-41CDB5B81BB2}" name="ornext" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{E2F5E83C-E84C-BE44-9D5C-411E6A9AEB7D}" name="message" dataDxfId="51"/>
-    <tableColumn id="8" xr3:uid="{C326F9E6-06E4-5440-9CE2-9ECA21575953}" name="type" dataDxfId="50"/>
-    <tableColumn id="9" xr3:uid="{DA813C67-D744-004E-BE75-F082CC056441}" name="url" dataDxfId="49"/>
-    <tableColumn id="10" xr3:uid="{DCC493DF-5EB5-3341-AEAA-9C51F3654086}" name="title" dataDxfId="48"/>
-    <tableColumn id="11" xr3:uid="{026EFC92-0438-5D4C-837D-0ADFC4FE2215}" name="description" dataDxfId="47"/>
-    <tableColumn id="12" xr3:uid="{8D251605-4659-7946-A0EE-C9390C5A6FC0}" name="section" dataDxfId="46"/>
-    <tableColumn id="13" xr3:uid="{B29E72DF-09C9-A546-A93D-814BA9931B2A}" name="sortorder" dataDxfId="45"/>
-    <tableColumn id="14" xr3:uid="{543C7DFD-FEBC-4343-B064-C44054889A42}" name="hidden" dataDxfId="44"/>
-    <tableColumn id="15" xr3:uid="{5B396502-6E5B-B44F-80BE-058D7DF9AC02}" name="rewards" dataDxfId="43"/>
-    <tableColumn id="16" xr3:uid="{167138EC-6CD6-D942-B86B-9B456F2F0697}" name="reset" dataDxfId="42"/>
-    <tableColumn id="17" xr3:uid="{71510075-C3B8-AA4F-85BF-5FF48A29D551}" name="jumpto" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{A9CB85C2-9EE9-E943-8583-198E332FFDDB}" name="label" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{ECEF0727-201A-294E-BD26-4AC0074C4525}" name="ifall" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{98DC9DDF-BDE6-8E4B-A641-1CA50F97B95E}" name="andnot" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{8BFB331E-5056-234D-86A1-1CBB34D2A4A4}" name="after" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{F7D28942-23E3-544B-AE2F-F73BE9CE5841}" name="waitfor" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{DE531C20-A3B2-5C46-A368-41CDB5B81BB2}" name="ornext" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{E2F5E83C-E84C-BE44-9D5C-411E6A9AEB7D}" name="message" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{C326F9E6-06E4-5440-9CE2-9ECA21575953}" name="type" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{DA813C67-D744-004E-BE75-F082CC056441}" name="url" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{DCC493DF-5EB5-3341-AEAA-9C51F3654086}" name="title" dataDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{026EFC92-0438-5D4C-837D-0ADFC4FE2215}" name="description" dataDxfId="42"/>
+    <tableColumn id="12" xr3:uid="{8D251605-4659-7946-A0EE-C9390C5A6FC0}" name="section" dataDxfId="41"/>
+    <tableColumn id="13" xr3:uid="{B29E72DF-09C9-A546-A93D-814BA9931B2A}" name="sortorder" dataDxfId="40"/>
+    <tableColumn id="14" xr3:uid="{543C7DFD-FEBC-4343-B064-C44054889A42}" name="hidden" dataDxfId="39"/>
+    <tableColumn id="15" xr3:uid="{5B396502-6E5B-B44F-80BE-058D7DF9AC02}" name="rewards" dataDxfId="38"/>
+    <tableColumn id="16" xr3:uid="{167138EC-6CD6-D942-B86B-9B456F2F0697}" name="reset" dataDxfId="37"/>
+    <tableColumn id="17" xr3:uid="{71510075-C3B8-AA4F-85BF-5FF48A29D551}" name="jumpto" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{257DB03E-7762-2242-B18E-58ACF3CAC862}" name="Table8106" displayName="Table8106" ref="A1:Q24" totalsRowShown="0" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{257DB03E-7762-2242-B18E-58ACF3CAC862}" name="Table8106" displayName="Table8106" ref="A1:Q24" totalsRowShown="0" dataDxfId="35">
   <autoFilter ref="A1:Q24" xr:uid="{669026F6-523A-EF49-B01A-F3286CFBC418}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{1E7C3318-FC2F-B147-A51B-4FD196F2957D}" name="label" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{C2AE6CBC-23AD-6343-ACE1-217D8E340B4A}" name="ifall" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{4C971A6D-0C29-0C45-BA39-BBCDA3E9E131}" name="andnot" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{B311C863-87CB-AA47-9825-411DC835E9E1}" name="after" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{E3B541D0-1685-1646-8BBB-C378E5E9C22B}" name="waitfor" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{A836FAC3-9EA9-6D46-957E-05F6E7E90A5F}" name="ornext" dataDxfId="34"/>
-    <tableColumn id="7" xr3:uid="{509DB9D9-B2D7-9544-B25B-250F74518FF0}" name="message" dataDxfId="33"/>
-    <tableColumn id="8" xr3:uid="{8B2796D2-CFF3-5A47-89B5-62D22485A4F7}" name="type" dataDxfId="32"/>
-    <tableColumn id="9" xr3:uid="{6916384F-C9DE-2141-A0CC-7261BB3C266B}" name="url" dataDxfId="31"/>
-    <tableColumn id="10" xr3:uid="{B711D3D3-3EC7-A743-93E1-2023C01BD30C}" name="title" dataDxfId="30"/>
-    <tableColumn id="11" xr3:uid="{AE04662E-664B-A14E-8293-9588D6C7B3B1}" name="description" dataDxfId="29"/>
-    <tableColumn id="12" xr3:uid="{1F8743AE-3940-9F4D-90F7-9E6CF355B1FF}" name="section" dataDxfId="28"/>
-    <tableColumn id="13" xr3:uid="{3E54C9A2-2F37-5244-AE63-B4D9127E0307}" name="sortorder" dataDxfId="27"/>
-    <tableColumn id="14" xr3:uid="{D96F5341-7EFD-7D40-8E28-2DB7E27BA2D7}" name="hidden" dataDxfId="26"/>
-    <tableColumn id="15" xr3:uid="{2718BFCD-4B8B-3A43-86A6-1BBC0F5A66E8}" name="rewards" dataDxfId="25"/>
-    <tableColumn id="16" xr3:uid="{6A98EB88-2159-BC47-AF38-E9F70BC7B160}" name="reset" dataDxfId="24"/>
-    <tableColumn id="17" xr3:uid="{600EFB22-3687-2441-BEEF-E4E2B5FF36FD}" name="jumpto" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{1E7C3318-FC2F-B147-A51B-4FD196F2957D}" name="label" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{C2AE6CBC-23AD-6343-ACE1-217D8E340B4A}" name="ifall" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{4C971A6D-0C29-0C45-BA39-BBCDA3E9E131}" name="andnot" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{B311C863-87CB-AA47-9825-411DC835E9E1}" name="after" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{E3B541D0-1685-1646-8BBB-C378E5E9C22B}" name="waitfor" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{A836FAC3-9EA9-6D46-957E-05F6E7E90A5F}" name="ornext" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{509DB9D9-B2D7-9544-B25B-250F74518FF0}" name="message" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{8B2796D2-CFF3-5A47-89B5-62D22485A4F7}" name="type" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{6916384F-C9DE-2141-A0CC-7261BB3C266B}" name="url" dataDxfId="26"/>
+    <tableColumn id="10" xr3:uid="{B711D3D3-3EC7-A743-93E1-2023C01BD30C}" name="title" dataDxfId="25"/>
+    <tableColumn id="11" xr3:uid="{AE04662E-664B-A14E-8293-9588D6C7B3B1}" name="description" dataDxfId="24"/>
+    <tableColumn id="12" xr3:uid="{1F8743AE-3940-9F4D-90F7-9E6CF355B1FF}" name="section" dataDxfId="23"/>
+    <tableColumn id="13" xr3:uid="{3E54C9A2-2F37-5244-AE63-B4D9127E0307}" name="sortorder" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{D96F5341-7EFD-7D40-8E28-2DB7E27BA2D7}" name="hidden" dataDxfId="21"/>
+    <tableColumn id="15" xr3:uid="{2718BFCD-4B8B-3A43-86A6-1BBC0F5A66E8}" name="rewards" dataDxfId="20"/>
+    <tableColumn id="16" xr3:uid="{6A98EB88-2159-BC47-AF38-E9F70BC7B160}" name="reset" dataDxfId="19"/>
+    <tableColumn id="17" xr3:uid="{600EFB22-3687-2441-BEEF-E4E2B5FF36FD}" name="jumpto" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1659,22 +1773,22 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" t="s">
         <v>77</v>
       </c>
-      <c r="E1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>67</v>
-      </c>
-      <c r="H1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I1" t="s">
-        <v>68</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -1682,13 +1796,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -1722,28 +1836,28 @@
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" t="s">
         <v>72</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1792,7 +1906,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -1801,22 +1915,22 @@
         <v>18</v>
       </c>
       <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
-        <v>37</v>
-      </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J1" t="s">
         <v>14</v>
@@ -1825,22 +1939,22 @@
         <v>1</v>
       </c>
       <c r="L1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M1" t="s">
         <v>19</v>
       </c>
       <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
         <v>41</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>42</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>43</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -1851,7 +1965,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -2327,46 +2441,46 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" t="s">
         <v>21</v>
       </c>
       <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
         <v>51</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>52</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>53</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>54</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>55</v>
       </c>
-      <c r="H28" t="s">
+      <c r="J28" t="s">
         <v>56</v>
       </c>
-      <c r="J28" t="s">
+      <c r="L28" t="s">
         <v>57</v>
-      </c>
-      <c r="L28" t="s">
-        <v>58</v>
       </c>
       <c r="N28" t="s">
         <v>5</v>
       </c>
       <c r="O28" t="s">
+        <v>58</v>
+      </c>
+      <c r="P28" t="s">
         <v>59</v>
       </c>
-      <c r="P28" t="s">
+      <c r="Q28" t="s">
         <v>60</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
@@ -2374,7 +2488,7 @@
         <v>3</v>
       </c>
       <c r="H29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N29" t="s">
         <v>3</v>
@@ -2385,7 +2499,7 @@
         <v>4</v>
       </c>
       <c r="H30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N30" t="s">
         <v>4</v>
@@ -2393,17 +2507,17 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2427,10 +2541,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA4BC58-8D9E-8247-A221-EA67BCFA1E88}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2466,53 +2580,51 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>89</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2520,7 +2632,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2528,7 +2640,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2536,31 +2648,43 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+        <v>135</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+        <v>136</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2568,95 +2692,93 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>136</v>
+        <v>179</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1" t="s">
-        <v>89</v>
-      </c>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2664,7 +2786,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2672,7 +2794,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2680,7 +2802,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2688,7 +2810,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2696,37 +2818,53 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>11</v>
-      </c>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>12</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>13</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C34" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2782,16 +2920,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -2801,14 +2939,14 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
@@ -2817,19 +2955,19 @@
         <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="3">
         <v>3</v>
@@ -2838,15 +2976,15 @@
         <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -2857,15 +2995,15 @@
         <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -2876,15 +3014,15 @@
         <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2895,15 +3033,15 @@
         <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -2911,7 +3049,7 @@
         <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -2935,7 +3073,7 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -2962,7 +3100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE9F943-FBE9-CA48-8381-FDD6A6E3E5D1}">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD11"/>
     </sheetView>
   </sheetViews>
@@ -2981,7 +3119,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -2990,22 +3128,22 @@
         <v>18</v>
       </c>
       <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
-        <v>37</v>
-      </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J1" t="s">
         <v>14</v>
@@ -3014,22 +3152,22 @@
         <v>1</v>
       </c>
       <c r="L1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M1" t="s">
         <v>19</v>
       </c>
       <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
         <v>41</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>42</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>43</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -3040,7 +3178,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -3061,7 +3199,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -3080,11 +3218,11 @@
       <c r="C4" s="1"/>
       <c r="D4" s="3"/>
       <c r="E4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -3524,46 +3662,46 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" t="s">
         <v>21</v>
       </c>
       <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
         <v>51</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>52</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>53</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>54</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>55</v>
       </c>
-      <c r="H28" t="s">
+      <c r="J28" t="s">
         <v>56</v>
       </c>
-      <c r="J28" t="s">
+      <c r="L28" t="s">
         <v>57</v>
-      </c>
-      <c r="L28" t="s">
-        <v>58</v>
       </c>
       <c r="N28" t="s">
         <v>5</v>
       </c>
       <c r="O28" t="s">
+        <v>58</v>
+      </c>
+      <c r="P28" t="s">
         <v>59</v>
       </c>
-      <c r="P28" t="s">
+      <c r="Q28" t="s">
         <v>60</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
@@ -3571,7 +3709,7 @@
         <v>3</v>
       </c>
       <c r="H29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N29" t="s">
         <v>3</v>
@@ -3582,7 +3720,7 @@
         <v>4</v>
       </c>
       <c r="H30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N30" t="s">
         <v>4</v>
@@ -3590,17 +3728,17 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -3643,7 +3781,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -3652,22 +3790,22 @@
         <v>18</v>
       </c>
       <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
-        <v>37</v>
-      </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J1" t="s">
         <v>14</v>
@@ -3676,22 +3814,22 @@
         <v>1</v>
       </c>
       <c r="L1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M1" t="s">
         <v>19</v>
       </c>
       <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
         <v>41</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>42</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>43</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -3702,7 +3840,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -3712,7 +3850,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -3725,7 +3863,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -3744,11 +3882,11 @@
       <c r="C4" s="1"/>
       <c r="D4" s="3"/>
       <c r="E4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -3758,10 +3896,10 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="Q4" s="1"/>
     </row>
@@ -4152,46 +4290,46 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
         <v>21</v>
       </c>
       <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
         <v>51</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>52</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>53</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>54</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>55</v>
       </c>
-      <c r="H26" t="s">
+      <c r="J26" t="s">
         <v>56</v>
       </c>
-      <c r="J26" t="s">
+      <c r="L26" t="s">
         <v>57</v>
-      </c>
-      <c r="L26" t="s">
-        <v>58</v>
       </c>
       <c r="N26" t="s">
         <v>5</v>
       </c>
       <c r="O26" t="s">
+        <v>58</v>
+      </c>
+      <c r="P26" t="s">
         <v>59</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>60</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
@@ -4199,7 +4337,7 @@
         <v>3</v>
       </c>
       <c r="H27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N27" t="s">
         <v>3</v>
@@ -4210,7 +4348,7 @@
         <v>4</v>
       </c>
       <c r="H28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N28" t="s">
         <v>4</v>
@@ -4218,17 +4356,17 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -4252,10 +4390,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B819C41-D178-6849-96F5-6846425DFC81}">
-  <dimension ref="A1:XFD36"/>
+  <dimension ref="A1:XFD67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4272,7 +4410,7 @@
   <sheetData>
     <row r="1" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -4281,22 +4419,22 @@
         <v>18</v>
       </c>
       <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
-        <v>37</v>
-      </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J1" t="s">
         <v>14</v>
@@ -4305,22 +4443,22 @@
         <v>1</v>
       </c>
       <c r="L1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M1" t="s">
         <v>19</v>
       </c>
       <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
         <v>41</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>42</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>43</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:16384" x14ac:dyDescent="0.2">
@@ -4331,7 +4469,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -4341,7 +4479,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -4354,7 +4492,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -4375,7 +4513,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -4391,7 +4529,7 @@
     <row r="5" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D5" s="3"/>
       <c r="E5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R5"/>
       <c r="S5"/>
@@ -20763,20 +20901,20 @@
     </row>
     <row r="6" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D6" s="3"/>
       <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="R6"/>
       <c r="S6"/>
@@ -37149,7 +37287,7 @@
     <row r="7" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D7" s="3"/>
       <c r="G7" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="R7"/>
       <c r="S7"/>
@@ -53523,16 +53661,18 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="1" t="s">
-        <v>106</v>
+        <v>181</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -53543,24 +53683,24 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="1" t="s">
-        <v>109</v>
+        <v>182</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -53570,28 +53710,28 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="1" t="s">
-        <v>110</v>
+        <v>183</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -53601,26 +53741,26 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="1" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>107</v>
+        <v>201</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -53629,20 +53769,18 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="O11" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1" t="s">
-        <v>108</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="3"/>
@@ -53659,11 +53797,11 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:16384" x14ac:dyDescent="0.2">
@@ -53674,7 +53812,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>112</v>
+        <v>186</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -53691,18 +53829,16 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>107</v>
-      </c>
+      <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -53710,23 +53846,21 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-      <c r="O14" s="1" t="s">
-        <v>142</v>
-      </c>
+      <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1" t="s">
-        <v>113</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>3</v>
@@ -53742,23 +53876,21 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="1" t="s">
-        <v>116</v>
+        <v>191</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="1" t="s">
-        <v>107</v>
-      </c>
+      <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -53766,17 +53898,15 @@
       <c r="L16" s="1"/>
       <c r="M16" s="3"/>
       <c r="N16" s="1"/>
-      <c r="O16" s="1" t="s">
-        <v>143</v>
-      </c>
+      <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1" t="s">
-        <v>113</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>117</v>
+        <v>188</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -53784,14 +53914,18 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+        <v>187</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>189</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="3"/>
+      <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -53805,55 +53939,60 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>119</v>
+        <v>190</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="3"/>
+      <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
-      <c r="XFD18" s="1"/>
     </row>
     <row r="19" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F19" s="1"/>
-      <c r="G19" s="1" t="s">
-        <v>120</v>
-      </c>
+      <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="3"/>
+      <c r="M19" s="1"/>
       <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
+      <c r="O19" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
+      <c r="Q19" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="20" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="3"/>
-      <c r="E20" t="s">
-        <v>62</v>
-      </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>220</v>
+      </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -53864,20 +54003,14 @@
       <c r="Q20" s="1"/>
     </row>
     <row r="21" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>125</v>
-      </c>
+      <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="3"/>
-      <c r="E21" t="s">
-        <v>122</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -53888,23 +54021,18 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
-      <c r="Q21" s="1" t="s">
-        <v>125</v>
-      </c>
+      <c r="Q21" s="1"/>
+      <c r="XFD21" s="1"/>
     </row>
     <row r="22" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="3"/>
-      <c r="E22" t="s">
-        <v>123</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -53913,13 +54041,9 @@
       <c r="L22" s="1"/>
       <c r="M22" s="3"/>
       <c r="N22" s="1"/>
-      <c r="O22" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="O22" s="1"/>
       <c r="P22" s="1"/>
-      <c r="Q22" s="1" t="s">
-        <v>113</v>
-      </c>
+      <c r="Q22" s="1"/>
     </row>
     <row r="23" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
@@ -53927,96 +54051,118 @@
       <c r="C23" s="1"/>
       <c r="D23" s="3"/>
       <c r="E23" t="s">
-        <v>124</v>
+        <v>61</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
+      <c r="M23" s="3"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
-      <c r="Q23" s="1" t="s">
-        <v>125</v>
-      </c>
+      <c r="Q23" s="1"/>
     </row>
     <row r="24" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="E24" t="s">
+        <v>113</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
+      <c r="M24" s="3"/>
       <c r="N24" s="1"/>
-      <c r="O24" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="25" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="E25" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
+      <c r="M25" s="3"/>
       <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
+      <c r="O25" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
+      <c r="Q25" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="26" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="5"/>
+      <c r="E26" t="s">
+        <v>115</v>
+      </c>
       <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="G26" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
-      <c r="M26" s="3"/>
+      <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
+      <c r="Q26" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="27" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>192</v>
+      </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="6"/>
+      <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="G27" s="1" t="s">
+        <v>193</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -54035,13 +54181,15 @@
       <c r="D28" s="3"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="G28" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
-      <c r="M28" s="3"/>
+      <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -54054,120 +54202,832 @@
       <c r="D29" s="3"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="G29" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
-      <c r="M29" s="3"/>
+      <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
     <row r="30" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>11</v>
-      </c>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
     </row>
     <row r="31" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" t="s">
-        <v>52</v>
-      </c>
-      <c r="E31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" t="s">
-        <v>54</v>
-      </c>
-      <c r="G31" t="s">
-        <v>55</v>
-      </c>
-      <c r="H31" t="s">
-        <v>56</v>
-      </c>
-      <c r="J31" t="s">
-        <v>57</v>
-      </c>
-      <c r="L31" t="s">
-        <v>58</v>
-      </c>
-      <c r="N31" t="s">
-        <v>5</v>
-      </c>
-      <c r="O31" t="s">
-        <v>59</v>
-      </c>
-      <c r="P31" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>61</v>
+      <c r="A31" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
-      <c r="F32" t="s">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H32" t="s">
+      <c r="G32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+    </row>
+    <row r="36" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N32" t="s">
+      <c r="I39" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+    </row>
+    <row r="40" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+    </row>
+    <row r="41" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+    </row>
+    <row r="43" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="XFD43" s="1"/>
+    </row>
+    <row r="44" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="3"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+    </row>
+    <row r="45" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="3"/>
+      <c r="E45" t="s">
+        <v>61</v>
+      </c>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+    </row>
+    <row r="47" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+    </row>
+    <row r="48" spans="1:17 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G50" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="33" spans="6:14" x14ac:dyDescent="0.2">
-      <c r="F33" t="s">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="P53" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q53" s="1"/>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>49</v>
+      </c>
+      <c r="B62" t="s">
+        <v>21</v>
+      </c>
+      <c r="C62" t="s">
+        <v>50</v>
+      </c>
+      <c r="D62" t="s">
+        <v>51</v>
+      </c>
+      <c r="E62" t="s">
+        <v>52</v>
+      </c>
+      <c r="F62" t="s">
+        <v>53</v>
+      </c>
+      <c r="G62" t="s">
+        <v>54</v>
+      </c>
+      <c r="H62" t="s">
+        <v>55</v>
+      </c>
+      <c r="J62" t="s">
+        <v>56</v>
+      </c>
+      <c r="L62" t="s">
+        <v>57</v>
+      </c>
+      <c r="N62" t="s">
+        <v>5</v>
+      </c>
+      <c r="O62" t="s">
+        <v>58</v>
+      </c>
+      <c r="P62" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="F63" t="s">
+        <v>3</v>
+      </c>
+      <c r="H63" t="s">
+        <v>44</v>
+      </c>
+      <c r="N63" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="F64" t="s">
         <v>4</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H64" t="s">
+        <v>45</v>
+      </c>
+      <c r="N64" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H65" t="s">
         <v>46</v>
       </c>
-      <c r="N33" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="34" spans="6:14" x14ac:dyDescent="0.2">
-      <c r="H34" t="s">
+    <row r="66" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H66" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="6:14" x14ac:dyDescent="0.2">
-      <c r="H35" t="s">
+    <row r="67" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H67" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="6:14" x14ac:dyDescent="0.2">
-      <c r="H36" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F29" xr:uid="{76AD0A2F-A7CC-894A-A42B-8DB053E4C857}">
-      <formula1>$F$32:$F$34</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F58:F60 F2:F55" xr:uid="{76AD0A2F-A7CC-894A-A42B-8DB053E4C857}">
+      <formula1>$F$63:$F$65</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H29" xr:uid="{DA7769CD-CF47-B440-8C33-3517F6C47958}">
-      <formula1>$H$32:$H$37</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H58:H60 H2:H55" xr:uid="{DA7769CD-CF47-B440-8C33-3517F6C47958}">
+      <formula1>$H$63:$H$68</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N29" xr:uid="{32472F5B-4163-5141-8278-FFBF242E8AA9}">
-      <formula1>$N$32:$N$34</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N58:N60 N2:N55" xr:uid="{32472F5B-4163-5141-8278-FFBF242E8AA9}">
+      <formula1>$N$63:$N$65</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="I17" r:id="rId1" xr:uid="{4F566931-78D9-F243-961A-529F55DE0F6B}"/>
+    <hyperlink ref="I39" r:id="rId2" xr:uid="{D23DE1C0-0269-A441-ABBA-ED31A46083D5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -54193,7 +55053,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -54202,22 +55062,22 @@
         <v>18</v>
       </c>
       <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
-        <v>37</v>
-      </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J1" t="s">
         <v>14</v>
@@ -54226,22 +55086,22 @@
         <v>1</v>
       </c>
       <c r="L1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M1" t="s">
         <v>19</v>
       </c>
       <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
         <v>41</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>42</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>43</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -54252,7 +55112,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -54262,7 +55122,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -54275,7 +55135,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -54294,11 +55154,11 @@
       <c r="C4" s="1"/>
       <c r="D4" s="3"/>
       <c r="E4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -54308,10 +55168,10 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="Q4" s="1"/>
     </row>
@@ -54702,46 +55562,46 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
         <v>21</v>
       </c>
       <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
         <v>51</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>52</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>53</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>54</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>55</v>
       </c>
-      <c r="H26" t="s">
+      <c r="J26" t="s">
         <v>56</v>
       </c>
-      <c r="J26" t="s">
+      <c r="L26" t="s">
         <v>57</v>
-      </c>
-      <c r="L26" t="s">
-        <v>58</v>
       </c>
       <c r="N26" t="s">
         <v>5</v>
       </c>
       <c r="O26" t="s">
+        <v>58</v>
+      </c>
+      <c r="P26" t="s">
         <v>59</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>60</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
@@ -54749,7 +55609,7 @@
         <v>3</v>
       </c>
       <c r="H27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N27" t="s">
         <v>3</v>
@@ -54760,7 +55620,7 @@
         <v>4</v>
       </c>
       <c r="H28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N28" t="s">
         <v>4</v>
@@ -54768,17 +55628,17 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -54821,7 +55681,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -54830,22 +55690,22 @@
         <v>18</v>
       </c>
       <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
-        <v>37</v>
-      </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J1" t="s">
         <v>14</v>
@@ -54854,22 +55714,22 @@
         <v>1</v>
       </c>
       <c r="L1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M1" t="s">
         <v>19</v>
       </c>
       <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
         <v>41</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>42</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>43</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -54880,7 +55740,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -54890,7 +55750,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -54903,7 +55763,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -54922,11 +55782,11 @@
       <c r="C4" s="1"/>
       <c r="D4" s="3"/>
       <c r="E4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -54936,10 +55796,10 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="Q4" s="1"/>
     </row>
@@ -55330,46 +56190,46 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
         <v>21</v>
       </c>
       <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
         <v>51</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>52</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>53</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>54</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>55</v>
       </c>
-      <c r="H26" t="s">
+      <c r="J26" t="s">
         <v>56</v>
       </c>
-      <c r="J26" t="s">
+      <c r="L26" t="s">
         <v>57</v>
-      </c>
-      <c r="L26" t="s">
-        <v>58</v>
       </c>
       <c r="N26" t="s">
         <v>5</v>
       </c>
       <c r="O26" t="s">
+        <v>58</v>
+      </c>
+      <c r="P26" t="s">
         <v>59</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>60</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
@@ -55377,7 +56237,7 @@
         <v>3</v>
       </c>
       <c r="H27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N27" t="s">
         <v>3</v>
@@ -55388,7 +56248,7 @@
         <v>4</v>
       </c>
       <c r="H28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N28" t="s">
         <v>4</v>
@@ -55396,17 +56256,17 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -55432,7 +56292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC23722-7275-9946-8E3B-4FA24E1CC520}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -55449,7 +56309,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -55458,22 +56318,22 @@
         <v>18</v>
       </c>
       <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
-        <v>37</v>
-      </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J1" t="s">
         <v>14</v>
@@ -55482,22 +56342,22 @@
         <v>1</v>
       </c>
       <c r="L1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M1" t="s">
         <v>19</v>
       </c>
       <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
         <v>41</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>42</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>43</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -55508,7 +56368,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -55518,7 +56378,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -55531,7 +56391,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -55546,10 +56406,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="3"/>
@@ -55558,7 +56418,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -55570,7 +56430,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -55581,7 +56441,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -55598,17 +56458,17 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -55618,28 +56478,28 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -55649,28 +56509,28 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -55680,28 +56540,28 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -55711,28 +56571,28 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -55742,28 +56602,28 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -55773,28 +56633,28 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -55804,26 +56664,26 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -55833,22 +56693,22 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="3"/>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -55862,12 +56722,12 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -55883,10 +56743,10 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="Q15" s="1"/>
     </row>
@@ -56087,46 +56947,46 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
         <v>21</v>
       </c>
       <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
         <v>51</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>52</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>53</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>54</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>55</v>
       </c>
-      <c r="H27" t="s">
+      <c r="J27" t="s">
         <v>56</v>
       </c>
-      <c r="J27" t="s">
+      <c r="L27" t="s">
         <v>57</v>
-      </c>
-      <c r="L27" t="s">
-        <v>58</v>
       </c>
       <c r="N27" t="s">
         <v>5</v>
       </c>
       <c r="O27" t="s">
+        <v>58</v>
+      </c>
+      <c r="P27" t="s">
         <v>59</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>60</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
@@ -56134,7 +56994,7 @@
         <v>3</v>
       </c>
       <c r="H28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N28" t="s">
         <v>3</v>
@@ -56145,7 +57005,7 @@
         <v>4</v>
       </c>
       <c r="H29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N29" t="s">
         <v>4</v>
@@ -56153,17 +57013,17 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>